<commit_message>
add: Apple + Google data
</commit_message>
<xml_diff>
--- a/02_Data/04_Social indicators/02_Cleaned Data/Population.xlsx
+++ b/02_Data/04_Social indicators/02_Cleaned Data/Population.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhachaichi\Documents\ESPON-DATA\02_Data\04_Social indicators\02_Cleaned Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76782094-22A9-4CB9-9387-326A4A4CAA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048FE612-14B1-4804-A573-3231EC15DC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,22 +25,220 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">Country </t>
-  </si>
-  <si>
-    <t xml:space="preserve">nuts_id </t>
-  </si>
-  <si>
-    <t>nuts_level</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
+  <si>
+    <t>Province of Namur</t>
+  </si>
+  <si>
+    <t>BE35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belgium </t>
+  </si>
+  <si>
+    <t>Province of Luxembourg</t>
+  </si>
+  <si>
+    <t>BE34</t>
+  </si>
+  <si>
+    <t>Province of Liège</t>
+  </si>
+  <si>
+    <t>BE33</t>
+  </si>
+  <si>
+    <t>Province of Hainaut</t>
+  </si>
+  <si>
+    <t>BE32</t>
+  </si>
+  <si>
+    <t>Province of Walloon Brabant</t>
+  </si>
+  <si>
+    <t>BE31</t>
+  </si>
+  <si>
+    <t>Province of West Flanders</t>
+  </si>
+  <si>
+    <t>BE25</t>
+  </si>
+  <si>
+    <t>Province of Flemish Brabant</t>
+  </si>
+  <si>
+    <t>BE24</t>
+  </si>
+  <si>
+    <t>Province of East Flanders</t>
+  </si>
+  <si>
+    <t>BE23</t>
+  </si>
+  <si>
+    <t>Province of Limburg</t>
+  </si>
+  <si>
+    <t>BE22</t>
+  </si>
+  <si>
+    <t>Province of Antwerp</t>
+  </si>
+  <si>
+    <t>BE21</t>
+  </si>
+  <si>
+    <t>Brussels-Capital Region</t>
+  </si>
+  <si>
+    <t>BE10</t>
+  </si>
+  <si>
+    <t>Norrbotten county</t>
+  </si>
+  <si>
+    <t>SE332</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden </t>
+  </si>
+  <si>
+    <t>Västerbotten county</t>
+  </si>
+  <si>
+    <t>SE331</t>
+  </si>
+  <si>
+    <t>Jämtland county</t>
+  </si>
+  <si>
+    <t>SE322</t>
+  </si>
+  <si>
+    <t>Västernorrland county</t>
+  </si>
+  <si>
+    <t>SE321</t>
+  </si>
+  <si>
+    <t>Gävleborg county</t>
+  </si>
+  <si>
+    <t>SE313</t>
+  </si>
+  <si>
+    <t>Dalarna county</t>
+  </si>
+  <si>
+    <t>SE312</t>
+  </si>
+  <si>
+    <t>Värmland county</t>
+  </si>
+  <si>
+    <t>SE311</t>
+  </si>
+  <si>
+    <t>Västra Götaland county</t>
+  </si>
+  <si>
+    <t>SE232</t>
+  </si>
+  <si>
+    <t>Halland county</t>
+  </si>
+  <si>
+    <t>SE231</t>
+  </si>
+  <si>
+    <t>Skåne county</t>
+  </si>
+  <si>
+    <t>SE224</t>
+  </si>
+  <si>
+    <t>Blekinge county</t>
+  </si>
+  <si>
+    <t>SE221</t>
+  </si>
+  <si>
+    <t>Gotland county</t>
+  </si>
+  <si>
+    <t>SE214</t>
+  </si>
+  <si>
+    <t>Kalmar county</t>
+  </si>
+  <si>
+    <t>SE213</t>
+  </si>
+  <si>
+    <t>Kronoberg county</t>
+  </si>
+  <si>
+    <t>SE212</t>
+  </si>
+  <si>
+    <t>Jönköping county</t>
+  </si>
+  <si>
+    <t>SE211</t>
+  </si>
+  <si>
+    <t>Västmanland county</t>
+  </si>
+  <si>
+    <t>SE125</t>
+  </si>
+  <si>
+    <t>Örebro county</t>
+  </si>
+  <si>
+    <t>SE124</t>
+  </si>
+  <si>
+    <t>Östergötland county</t>
+  </si>
+  <si>
+    <t>SE123</t>
+  </si>
+  <si>
+    <t>Södermanland county</t>
+  </si>
+  <si>
+    <t>SE122</t>
+  </si>
+  <si>
+    <t>Uppsala county</t>
+  </si>
+  <si>
+    <t>SE121</t>
+  </si>
+  <si>
+    <t>Stockholm county</t>
+  </si>
+  <si>
+    <t>SE110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country </t>
+  </si>
+  <si>
+    <t>nuts_id</t>
+  </si>
+  <si>
+    <t>nuts_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,6 +253,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,15 +285,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{B9650467-9FBE-440D-A31E-D356266C1AB5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -360,32 +575,540 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2020</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2391841</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2411859</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="2">
+        <v>388076</v>
+      </c>
+      <c r="E3" s="2">
+        <v>394154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="2">
+        <v>299329</v>
+      </c>
+      <c r="E4" s="2">
+        <v>301382</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="2">
+        <v>467276</v>
+      </c>
+      <c r="E5" s="2">
+        <v>469445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2">
+        <v>305715</v>
+      </c>
+      <c r="E6" s="2">
+        <v>306688</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2">
+        <v>277228</v>
+      </c>
+      <c r="E7" s="2">
+        <v>278721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="2">
+        <v>364953</v>
+      </c>
+      <c r="E8" s="2">
+        <v>366840</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="2">
+        <v>202247</v>
+      </c>
+      <c r="E9" s="2">
+        <v>203243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2">
+        <v>246033</v>
+      </c>
+      <c r="E10" s="2">
+        <v>246989</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="2">
+        <v>60050</v>
+      </c>
+      <c r="E11" s="2">
+        <v>60972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2">
+        <v>159227</v>
+      </c>
+      <c r="E12" s="2">
+        <v>158999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1388910</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1400973</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2">
+        <v>336440</v>
+      </c>
+      <c r="E14" s="2">
+        <v>339903</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1734344</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1743304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="2">
+        <v>282906</v>
+      </c>
+      <c r="E16" s="2">
+        <v>283169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="2">
+        <v>287681</v>
+      </c>
+      <c r="E17" s="2">
+        <v>288164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2">
+        <v>287631</v>
+      </c>
+      <c r="E18" s="2">
+        <v>287873</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2">
+        <v>244663</v>
+      </c>
+      <c r="E19" s="2">
+        <v>244223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="2">
+        <v>131064</v>
+      </c>
+      <c r="E20" s="2">
+        <v>131914</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="2">
+        <v>273220</v>
+      </c>
+      <c r="E21" s="2">
+        <v>274533</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="2">
+        <v>249649</v>
+      </c>
+      <c r="E22" s="2">
+        <v>249752</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>1219970</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24">
+        <v>1875524</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25">
+        <v>880397</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>1531745</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27">
+        <v>1162084</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>1203312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>407397</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>1345947</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>1109067</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>288722</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2020</v>
-      </c>
-      <c r="F1" s="1">
-        <v>2021</v>
+      <c r="D33">
+        <v>497073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>